<commit_message>
planilha  de sprint atualizada #3
</commit_message>
<xml_diff>
--- a/Documentação/Project Backlog.xlsx
+++ b/Documentação/Project Backlog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\projeto\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EFECA0-21D5-460B-8696-63AF3BBC0C04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="5" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint BandTec (2°)'!$A$1:$D$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="228">
   <si>
     <t>id</t>
   </si>
@@ -720,12 +719,15 @@
   </si>
   <si>
     <t>Pesquisar Dashboard do projeto @JP</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1410,57 +1412,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1474,6 +1425,57 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1787,7 +1789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809286DD-D5C9-4F7B-AD94-6A53F56382A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1822,7 +1824,7 @@
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="91" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1839,7 +1841,7 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="85"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="5" t="s">
         <v>50</v>
       </c>
@@ -1854,7 +1856,7 @@
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="85"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
@@ -1869,7 +1871,7 @@
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="85"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1884,7 +1886,7 @@
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="85"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="5" t="s">
         <v>56</v>
       </c>
@@ -1899,7 +1901,7 @@
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="85"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="6" t="s">
         <v>58</v>
       </c>
@@ -1914,7 +1916,7 @@
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="85"/>
+      <c r="B8" s="92"/>
       <c r="C8" s="5" t="s">
         <v>60</v>
       </c>
@@ -1929,7 +1931,7 @@
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="86"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="21" t="s">
         <v>62</v>
       </c>
@@ -1968,7 +1970,7 @@
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="91" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1985,7 +1987,7 @@
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="85"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="5" t="s">
         <v>67</v>
       </c>
@@ -2000,7 +2002,7 @@
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="85"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="5" t="s">
         <v>69</v>
       </c>
@@ -2015,7 +2017,7 @@
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="85"/>
+      <c r="B15" s="92"/>
       <c r="C15" s="5" t="s">
         <v>71</v>
       </c>
@@ -2030,7 +2032,7 @@
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="5" t="s">
         <v>77</v>
       </c>
@@ -2045,7 +2047,7 @@
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="85"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
@@ -2060,7 +2062,7 @@
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="85"/>
+      <c r="B18" s="92"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
@@ -2075,7 +2077,7 @@
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="86"/>
+      <c r="B19" s="93"/>
       <c r="C19" s="21" t="s">
         <v>75</v>
       </c>
@@ -2108,7 +2110,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="91" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2125,7 +2127,7 @@
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="85"/>
+      <c r="B23" s="92"/>
       <c r="C23" s="5" t="s">
         <v>82</v>
       </c>
@@ -2140,7 +2142,7 @@
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="85"/>
+      <c r="B24" s="92"/>
       <c r="C24" s="5" t="s">
         <v>84</v>
       </c>
@@ -2155,7 +2157,7 @@
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="85"/>
+      <c r="B25" s="92"/>
       <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
@@ -2170,7 +2172,7 @@
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="85"/>
+      <c r="B26" s="92"/>
       <c r="C26" s="5" t="s">
         <v>88</v>
       </c>
@@ -2185,7 +2187,7 @@
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="85"/>
+      <c r="B27" s="92"/>
       <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
@@ -2208,7 +2210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1AC4D2-7026-4F35-A980-9AD1E4D216BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -2243,7 +2245,7 @@
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="95" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="81" t="s">
@@ -2260,7 +2262,7 @@
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="88"/>
+      <c r="B3" s="95"/>
       <c r="C3" s="6" t="s">
         <v>186</v>
       </c>
@@ -2276,7 +2278,7 @@
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="6" t="s">
         <v>187</v>
       </c>
@@ -2292,7 +2294,7 @@
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="88"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="6" t="s">
         <v>188</v>
       </c>
@@ -2307,7 +2309,7 @@
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="88"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="6" t="s">
         <v>189</v>
       </c>
@@ -2322,7 +2324,7 @@
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="89"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="28" t="s">
         <v>190</v>
       </c>
@@ -2344,7 +2346,7 @@
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="94" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2361,7 +2363,7 @@
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="35" t="s">
         <v>193</v>
       </c>
@@ -2376,7 +2378,7 @@
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="6" t="s">
         <v>194</v>
       </c>
@@ -2391,7 +2393,7 @@
       <c r="A12" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="88"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="5" t="s">
         <v>99</v>
       </c>
@@ -2406,7 +2408,7 @@
       <c r="A13" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="88"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="6" t="s">
         <v>195</v>
       </c>
@@ -2421,7 +2423,7 @@
       <c r="A14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="88"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="6" t="s">
         <v>196</v>
       </c>
@@ -2436,7 +2438,7 @@
       <c r="A15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="88"/>
+      <c r="B15" s="95"/>
       <c r="C15" s="6" t="s">
         <v>102</v>
       </c>
@@ -2451,7 +2453,7 @@
       <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="95"/>
       <c r="C16" s="6" t="s">
         <v>198</v>
       </c>
@@ -2466,7 +2468,7 @@
       <c r="A17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="88"/>
+      <c r="B17" s="95"/>
       <c r="C17" s="6" t="s">
         <v>199</v>
       </c>
@@ -2481,7 +2483,7 @@
       <c r="A18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="88"/>
+      <c r="B18" s="95"/>
       <c r="C18" s="6" t="s">
         <v>201</v>
       </c>
@@ -2496,7 +2498,7 @@
       <c r="A19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="88"/>
+      <c r="B19" s="95"/>
       <c r="C19" s="6" t="s">
         <v>202</v>
       </c>
@@ -2511,7 +2513,7 @@
       <c r="A20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="88"/>
+      <c r="B20" s="95"/>
       <c r="C20" s="6" t="s">
         <v>107</v>
       </c>
@@ -2526,7 +2528,7 @@
       <c r="A21" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="88"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="6" t="s">
         <v>200</v>
       </c>
@@ -2541,7 +2543,7 @@
       <c r="A22" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="6" t="s">
         <v>110</v>
       </c>
@@ -2556,7 +2558,7 @@
       <c r="A23" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="88"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="6" t="s">
         <v>203</v>
       </c>
@@ -2571,7 +2573,7 @@
       <c r="A24" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="88"/>
+      <c r="B24" s="95"/>
       <c r="C24" s="6" t="s">
         <v>204</v>
       </c>
@@ -2586,7 +2588,7 @@
       <c r="A25" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="88"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="6" t="s">
         <v>205</v>
       </c>
@@ -2601,7 +2603,7 @@
       <c r="A26" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="88"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="6" t="s">
         <v>206</v>
       </c>
@@ -2616,7 +2618,7 @@
       <c r="A27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="88"/>
+      <c r="B27" s="95"/>
       <c r="C27" s="6" t="s">
         <v>207</v>
       </c>
@@ -2631,7 +2633,7 @@
       <c r="A28" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="88"/>
+      <c r="B28" s="95"/>
       <c r="C28" s="6" t="s">
         <v>208</v>
       </c>
@@ -2646,7 +2648,7 @@
       <c r="A29" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="88"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="6" t="s">
         <v>209</v>
       </c>
@@ -2661,7 +2663,7 @@
       <c r="A30" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="88"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="6" t="s">
         <v>210</v>
       </c>
@@ -2676,7 +2678,7 @@
       <c r="A31" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="88"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="35" t="s">
         <v>118</v>
       </c>
@@ -2691,7 +2693,7 @@
       <c r="A32" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="88"/>
+      <c r="B32" s="95"/>
       <c r="C32" s="5" t="s">
         <v>211</v>
       </c>
@@ -2706,7 +2708,7 @@
       <c r="A33" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="88"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="6" t="s">
         <v>213</v>
       </c>
@@ -2721,7 +2723,7 @@
       <c r="A34" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="88"/>
+      <c r="B34" s="95"/>
       <c r="C34" s="5" t="s">
         <v>212</v>
       </c>
@@ -2736,7 +2738,7 @@
       <c r="A35" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="88"/>
+      <c r="B35" s="95"/>
       <c r="C35" s="6" t="s">
         <v>214</v>
       </c>
@@ -2751,7 +2753,7 @@
       <c r="A36" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="95"/>
       <c r="C36" s="6" t="s">
         <v>215</v>
       </c>
@@ -2766,7 +2768,7 @@
       <c r="A37" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="89"/>
+      <c r="B37" s="96"/>
       <c r="C37" s="28" t="s">
         <v>216</v>
       </c>
@@ -2788,7 +2790,7 @@
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="94" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -2805,7 +2807,7 @@
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="88"/>
+      <c r="B40" s="95"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
@@ -2820,7 +2822,7 @@
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="89"/>
+      <c r="B41" s="96"/>
       <c r="C41" s="21" t="s">
         <v>124</v>
       </c>
@@ -2842,7 +2844,7 @@
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="87" t="s">
+      <c r="B43" s="94" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2859,7 +2861,7 @@
       <c r="A44" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="88"/>
+      <c r="B44" s="95"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2874,7 +2876,7 @@
       <c r="A45" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="89"/>
+      <c r="B45" s="96"/>
       <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
@@ -2886,7 +2888,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E7" xr:uid="{865F9192-6108-4E15-B8CE-16C6CF59E4A9}"/>
+  <autoFilter ref="A1:E7"/>
   <sortState ref="A3:A41">
     <sortCondition ref="A2"/>
   </sortState>
@@ -2902,7 +2904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368B4F2A-840E-43DD-A714-BED4E8CCE39E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2934,7 +2936,7 @@
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="97" t="s">
         <v>151</v>
       </c>
       <c r="C2" s="65" t="s">
@@ -2948,7 +2950,7 @@
       <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="91"/>
+      <c r="B3" s="98"/>
       <c r="C3" s="66" t="s">
         <v>153</v>
       </c>
@@ -2960,7 +2962,7 @@
       <c r="A4" s="45">
         <v>3</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="97" t="s">
         <v>154</v>
       </c>
       <c r="C4" s="65" t="s">
@@ -2974,7 +2976,7 @@
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="63" t="s">
         <v>156</v>
       </c>
@@ -2986,7 +2988,7 @@
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="91"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="66" t="s">
         <v>157</v>
       </c>
@@ -2998,7 +3000,7 @@
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="97" t="s">
         <v>158</v>
       </c>
       <c r="C7" s="65" t="s">
@@ -3012,7 +3014,7 @@
       <c r="A8" s="46">
         <v>7</v>
       </c>
-      <c r="B8" s="92"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="63" t="s">
         <v>160</v>
       </c>
@@ -3024,7 +3026,7 @@
       <c r="A9" s="48">
         <v>8</v>
       </c>
-      <c r="B9" s="91"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="66" t="s">
         <v>161</v>
       </c>
@@ -3036,7 +3038,7 @@
       <c r="A10" s="45">
         <v>9</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="97" t="s">
         <v>162</v>
       </c>
       <c r="C10" s="65" t="s">
@@ -3050,7 +3052,7 @@
       <c r="A11" s="48">
         <v>10</v>
       </c>
-      <c r="B11" s="91"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="66" t="s">
         <v>164</v>
       </c>
@@ -3062,7 +3064,7 @@
       <c r="A12" s="45">
         <v>11</v>
       </c>
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="97" t="s">
         <v>165</v>
       </c>
       <c r="C12" s="65" t="s">
@@ -3076,7 +3078,7 @@
       <c r="A13" s="46">
         <v>12</v>
       </c>
-      <c r="B13" s="92"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="63" t="s">
         <v>167</v>
       </c>
@@ -3088,7 +3090,7 @@
       <c r="A14" s="48">
         <v>13</v>
       </c>
-      <c r="B14" s="91"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="66" t="s">
         <v>168</v>
       </c>
@@ -3097,7 +3099,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D14" xr:uid="{161861C5-1A09-434C-804D-30DFA2AAE944}"/>
+  <autoFilter ref="A1:D14"/>
   <mergeCells count="5">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
@@ -3111,7 +3113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB8FA7D-215A-423D-A0CE-12EFD18E3EEC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3143,7 +3145,7 @@
       <c r="A2" s="52">
         <v>1</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="100" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="76" t="s">
@@ -3158,7 +3160,7 @@
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="77" t="s">
         <v>174</v>
       </c>
@@ -3170,7 +3172,7 @@
       <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="77" t="s">
         <v>175</v>
       </c>
@@ -3182,7 +3184,7 @@
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="77" t="s">
         <v>176</v>
       </c>
@@ -3194,7 +3196,7 @@
       <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="77" t="s">
         <v>177</v>
       </c>
@@ -3206,7 +3208,7 @@
       <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="91"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="57" t="s">
         <v>178</v>
       </c>
@@ -3218,7 +3220,7 @@
       <c r="A8" s="45">
         <v>8</v>
       </c>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="101" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="78" t="s">
@@ -3232,7 +3234,7 @@
       <c r="A9" s="48">
         <v>7</v>
       </c>
-      <c r="B9" s="95"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="57" t="s">
         <v>180</v>
       </c>
@@ -3255,7 +3257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC1D336-9D64-4429-8CDB-FA9C7AC22479}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3287,7 +3289,7 @@
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="103" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="79" t="s">
@@ -3301,7 +3303,7 @@
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
+      <c r="B3" s="104"/>
       <c r="C3" s="77" t="s">
         <v>217</v>
       </c>
@@ -3313,7 +3315,7 @@
       <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="98"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="57" t="s">
         <v>218</v>
       </c>
@@ -3325,7 +3327,7 @@
       <c r="A5" s="45">
         <v>4</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="101" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="78" t="s">
@@ -3339,7 +3341,7 @@
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="102"/>
       <c r="C6" s="57" t="s">
         <v>183</v>
       </c>
@@ -3351,7 +3353,7 @@
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="101" t="s">
         <v>150</v>
       </c>
       <c r="C7" s="80" t="s">
@@ -3365,7 +3367,7 @@
       <c r="A8" s="48">
         <v>7</v>
       </c>
-      <c r="B8" s="95"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="82" t="s">
         <v>185</v>
       </c>
@@ -3384,11 +3386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CBAEDD-70F6-4935-AB4E-56CD08B3DFA4}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,7 +3400,7 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>149</v>
       </c>
@@ -3412,11 +3414,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="106" t="s">
         <v>219</v>
       </c>
       <c r="C2" s="83" t="s">
@@ -3426,11 +3428,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="100"/>
+      <c r="B3" s="107"/>
       <c r="C3" s="77" t="s">
         <v>225</v>
       </c>
@@ -3438,11 +3440,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="107"/>
       <c r="C4" s="77" t="s">
         <v>221</v>
       </c>
@@ -3450,11 +3452,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="77" t="s">
         <v>222</v>
       </c>
@@ -3462,11 +3464,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="77" t="s">
         <v>223</v>
       </c>
@@ -3474,29 +3476,32 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101">
+    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="84">
         <v>6</v>
       </c>
-      <c r="B7" s="100"/>
-      <c r="C7" s="102" t="s">
+      <c r="B7" s="107"/>
+      <c r="C7" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D7" s="86" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="104">
+      <c r="E7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="87">
         <v>7</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="106" t="s">
+      <c r="C8" s="89" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="90" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sprint backlog da semana e tutorial nodeJS
</commit_message>
<xml_diff>
--- a/Documentação/Project Backlog.xlsx
+++ b/Documentação/Project Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\projeto\boxzard\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68F4999-7ED8-4FBA-85C4-EE444EC1B400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -18,6 +19,7 @@
     <sheet name="Sprint Backlog (29-03)" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint Backlog (04-04)" sheetId="4" r:id="rId5"/>
     <sheet name="Sprint Backlog (09-04)" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint Backlog (19-04)" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
@@ -28,17 +30,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="235">
   <si>
     <t>id</t>
   </si>
@@ -721,13 +718,34 @@
     <t>Pesquisar Dashboard do projeto @JP</t>
   </si>
   <si>
-    <t>OK</t>
+    <t>Fazer modal com opções de edição de produto, ambiente e informações dos galpões na página galpões.</t>
+  </si>
+  <si>
+    <t>Alinhar cores das páginas já feitas e as conectar por links.</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
+    <t>Inserir dados consistentes no banco de dados relacionados a usuários e galpões.</t>
+  </si>
+  <si>
+    <t>Testar querys de select com as informações inseridas no banco de dados.</t>
+  </si>
+  <si>
+    <t>Fazer barra de menu lateral para navegação entre as páginas do site.</t>
+  </si>
+  <si>
+    <t>Fazer tutorial de nodeJS para professora Marise.</t>
+  </si>
+  <si>
+    <t>Revisar planilha de riscos do projeto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1255,7 +1273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1476,6 +1494,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1789,7 +1814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2210,7 +2235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -2888,7 +2913,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E7"/>
+  <autoFilter ref="A1:E7" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <sortState ref="A3:A41">
     <sortCondition ref="A2"/>
   </sortState>
@@ -2904,7 +2929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3099,7 +3124,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D14"/>
+  <autoFilter ref="A1:D14" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="5">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
@@ -3113,7 +3138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3257,10 +3282,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -3386,11 +3411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,7 +3425,7 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>149</v>
       </c>
@@ -3414,7 +3439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -3428,7 +3453,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>2</v>
       </c>
@@ -3440,7 +3465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="46">
         <v>3</v>
       </c>
@@ -3452,7 +3477,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>4</v>
       </c>
@@ -3464,7 +3489,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>5</v>
       </c>
@@ -3476,7 +3501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="84">
         <v>6</v>
       </c>
@@ -3487,11 +3512,8 @@
       <c r="D7" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="87">
         <v>7</v>
       </c>
@@ -3511,4 +3533,133 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9C175-D83D-4C5E-A56D-A8DC851B7CF5}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
+        <v>2</v>
+      </c>
+      <c r="B3" s="108"/>
+      <c r="C3" s="77" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="84">
+        <v>3</v>
+      </c>
+      <c r="B4" s="109"/>
+      <c r="C4" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="45">
+        <v>4</v>
+      </c>
+      <c r="B5" s="103" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="79" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84">
+        <v>5</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="85" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="45">
+        <v>6</v>
+      </c>
+      <c r="B7" s="101" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="110">
+        <v>7</v>
+      </c>
+      <c r="B8" s="102"/>
+      <c r="C8" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Project Backlog e Atualização páginas internas system
</commit_message>
<xml_diff>
--- a/Documentação/Project Backlog.xlsx
+++ b/Documentação/Project Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68F4999-7ED8-4FBA-85C4-EE444EC1B400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2D743F-7926-474A-BA25-316B6941CF28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Sprint Backlog (29-03)" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint Backlog (04-04)" sheetId="4" r:id="rId5"/>
     <sheet name="Sprint Backlog (09-04)" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint Backlog (19-04)" sheetId="7" r:id="rId7"/>
+    <sheet name="Sprint Backlog (18-04)" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
@@ -1443,6 +1443,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1500,7 +1501,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1849,7 +1849,7 @@
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="92" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1866,7 +1866,7 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
+      <c r="B3" s="93"/>
       <c r="C3" s="5" t="s">
         <v>50</v>
       </c>
@@ -1881,7 +1881,7 @@
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
@@ -1896,7 +1896,7 @@
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1911,7 +1911,7 @@
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="5" t="s">
         <v>56</v>
       </c>
@@ -1926,7 +1926,7 @@
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="92"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="6" t="s">
         <v>58</v>
       </c>
@@ -1941,7 +1941,7 @@
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="92"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="5" t="s">
         <v>60</v>
       </c>
@@ -1956,7 +1956,7 @@
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="93"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="21" t="s">
         <v>62</v>
       </c>
@@ -1995,7 +1995,7 @@
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="92" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2012,7 +2012,7 @@
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="92"/>
+      <c r="B13" s="93"/>
       <c r="C13" s="5" t="s">
         <v>67</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="92"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="5" t="s">
         <v>69</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="92"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="5" t="s">
         <v>71</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="92"/>
+      <c r="B16" s="93"/>
       <c r="C16" s="5" t="s">
         <v>77</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="92"/>
+      <c r="B17" s="93"/>
       <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
@@ -2087,7 +2087,7 @@
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="92"/>
+      <c r="B18" s="93"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
@@ -2102,7 +2102,7 @@
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="93"/>
+      <c r="B19" s="94"/>
       <c r="C19" s="21" t="s">
         <v>75</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="92" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2152,7 +2152,7 @@
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="92"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="5" t="s">
         <v>82</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="92"/>
+      <c r="B24" s="93"/>
       <c r="C24" s="5" t="s">
         <v>84</v>
       </c>
@@ -2182,7 +2182,7 @@
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="92"/>
+      <c r="B25" s="93"/>
       <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="92"/>
+      <c r="B26" s="93"/>
       <c r="C26" s="5" t="s">
         <v>88</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="92"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
@@ -2270,7 +2270,7 @@
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="81" t="s">
@@ -2287,7 +2287,7 @@
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="95"/>
+      <c r="B3" s="96"/>
       <c r="C3" s="6" t="s">
         <v>186</v>
       </c>
@@ -2303,7 +2303,7 @@
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="6" t="s">
         <v>187</v>
       </c>
@@ -2319,7 +2319,7 @@
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="95"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="6" t="s">
         <v>188</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="6" t="s">
         <v>189</v>
       </c>
@@ -2349,7 +2349,7 @@
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="28" t="s">
         <v>190</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="95" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2388,7 +2388,7 @@
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="95"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="35" t="s">
         <v>193</v>
       </c>
@@ -2403,7 +2403,7 @@
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="95"/>
+      <c r="B11" s="96"/>
       <c r="C11" s="6" t="s">
         <v>194</v>
       </c>
@@ -2418,7 +2418,7 @@
       <c r="A12" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="95"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="5" t="s">
         <v>99</v>
       </c>
@@ -2433,7 +2433,7 @@
       <c r="A13" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="95"/>
+      <c r="B13" s="96"/>
       <c r="C13" s="6" t="s">
         <v>195</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="A14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="95"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="6" t="s">
         <v>196</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="A15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="95"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="6" t="s">
         <v>102</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="95"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="6" t="s">
         <v>198</v>
       </c>
@@ -2493,7 +2493,7 @@
       <c r="A17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="95"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="6" t="s">
         <v>199</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="A18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="95"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="6" t="s">
         <v>201</v>
       </c>
@@ -2523,7 +2523,7 @@
       <c r="A19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="95"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="6" t="s">
         <v>202</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="A20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="95"/>
+      <c r="B20" s="96"/>
       <c r="C20" s="6" t="s">
         <v>107</v>
       </c>
@@ -2553,7 +2553,7 @@
       <c r="A21" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="95"/>
+      <c r="B21" s="96"/>
       <c r="C21" s="6" t="s">
         <v>200</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="A22" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="95"/>
+      <c r="B22" s="96"/>
       <c r="C22" s="6" t="s">
         <v>110</v>
       </c>
@@ -2583,7 +2583,7 @@
       <c r="A23" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="95"/>
+      <c r="B23" s="96"/>
       <c r="C23" s="6" t="s">
         <v>203</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="A24" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="95"/>
+      <c r="B24" s="96"/>
       <c r="C24" s="6" t="s">
         <v>204</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="A25" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="95"/>
+      <c r="B25" s="96"/>
       <c r="C25" s="6" t="s">
         <v>205</v>
       </c>
@@ -2628,7 +2628,7 @@
       <c r="A26" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="95"/>
+      <c r="B26" s="96"/>
       <c r="C26" s="6" t="s">
         <v>206</v>
       </c>
@@ -2643,7 +2643,7 @@
       <c r="A27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="95"/>
+      <c r="B27" s="96"/>
       <c r="C27" s="6" t="s">
         <v>207</v>
       </c>
@@ -2658,7 +2658,7 @@
       <c r="A28" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="95"/>
+      <c r="B28" s="96"/>
       <c r="C28" s="6" t="s">
         <v>208</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="A29" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="95"/>
+      <c r="B29" s="96"/>
       <c r="C29" s="6" t="s">
         <v>209</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="A30" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="95"/>
+      <c r="B30" s="96"/>
       <c r="C30" s="6" t="s">
         <v>210</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="A31" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="95"/>
+      <c r="B31" s="96"/>
       <c r="C31" s="35" t="s">
         <v>118</v>
       </c>
@@ -2718,7 +2718,7 @@
       <c r="A32" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="95"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="5" t="s">
         <v>211</v>
       </c>
@@ -2733,7 +2733,7 @@
       <c r="A33" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="95"/>
+      <c r="B33" s="96"/>
       <c r="C33" s="6" t="s">
         <v>213</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="A34" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="95"/>
+      <c r="B34" s="96"/>
       <c r="C34" s="5" t="s">
         <v>212</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="A35" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="95"/>
+      <c r="B35" s="96"/>
       <c r="C35" s="6" t="s">
         <v>214</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="A36" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="95"/>
+      <c r="B36" s="96"/>
       <c r="C36" s="6" t="s">
         <v>215</v>
       </c>
@@ -2793,7 +2793,7 @@
       <c r="A37" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="96"/>
+      <c r="B37" s="97"/>
       <c r="C37" s="28" t="s">
         <v>216</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="95" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -2832,7 +2832,7 @@
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="95"/>
+      <c r="B40" s="96"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="96"/>
+      <c r="B41" s="97"/>
       <c r="C41" s="21" t="s">
         <v>124</v>
       </c>
@@ -2869,7 +2869,7 @@
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="95" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2886,7 +2886,7 @@
       <c r="A44" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="95"/>
+      <c r="B44" s="96"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="A45" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="96"/>
+      <c r="B45" s="97"/>
       <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
@@ -2961,7 +2961,7 @@
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="98" t="s">
         <v>151</v>
       </c>
       <c r="C2" s="65" t="s">
@@ -2975,7 +2975,7 @@
       <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="98"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="66" t="s">
         <v>153</v>
       </c>
@@ -2987,7 +2987,7 @@
       <c r="A4" s="45">
         <v>3</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="98" t="s">
         <v>154</v>
       </c>
       <c r="C4" s="65" t="s">
@@ -3001,7 +3001,7 @@
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="99"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="63" t="s">
         <v>156</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="98"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="66" t="s">
         <v>157</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="98" t="s">
         <v>158</v>
       </c>
       <c r="C7" s="65" t="s">
@@ -3039,7 +3039,7 @@
       <c r="A8" s="46">
         <v>7</v>
       </c>
-      <c r="B8" s="99"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="63" t="s">
         <v>160</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="A9" s="48">
         <v>8</v>
       </c>
-      <c r="B9" s="98"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="66" t="s">
         <v>161</v>
       </c>
@@ -3063,7 +3063,7 @@
       <c r="A10" s="45">
         <v>9</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="98" t="s">
         <v>162</v>
       </c>
       <c r="C10" s="65" t="s">
@@ -3077,7 +3077,7 @@
       <c r="A11" s="48">
         <v>10</v>
       </c>
-      <c r="B11" s="98"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="66" t="s">
         <v>164</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="A12" s="45">
         <v>11</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="98" t="s">
         <v>165</v>
       </c>
       <c r="C12" s="65" t="s">
@@ -3103,7 +3103,7 @@
       <c r="A13" s="46">
         <v>12</v>
       </c>
-      <c r="B13" s="99"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="63" t="s">
         <v>167</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="A14" s="48">
         <v>13</v>
       </c>
-      <c r="B14" s="98"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="66" t="s">
         <v>168</v>
       </c>
@@ -3170,7 +3170,7 @@
       <c r="A2" s="52">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="101" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="76" t="s">
@@ -3185,7 +3185,7 @@
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="99"/>
+      <c r="B3" s="100"/>
       <c r="C3" s="77" t="s">
         <v>174</v>
       </c>
@@ -3197,7 +3197,7 @@
       <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="77" t="s">
         <v>175</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="99"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="77" t="s">
         <v>176</v>
       </c>
@@ -3221,7 +3221,7 @@
       <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="99"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="77" t="s">
         <v>177</v>
       </c>
@@ -3233,7 +3233,7 @@
       <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="98"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="57" t="s">
         <v>178</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="A8" s="45">
         <v>8</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="102" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="78" t="s">
@@ -3259,7 +3259,7 @@
       <c r="A9" s="48">
         <v>7</v>
       </c>
-      <c r="B9" s="102"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="57" t="s">
         <v>180</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="104" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="79" t="s">
@@ -3328,7 +3328,7 @@
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="104"/>
+      <c r="B3" s="105"/>
       <c r="C3" s="77" t="s">
         <v>217</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="105"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="57" t="s">
         <v>218</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="A5" s="45">
         <v>4</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="102" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="78" t="s">
@@ -3366,7 +3366,7 @@
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="102"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="57" t="s">
         <v>183</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="102" t="s">
         <v>150</v>
       </c>
       <c r="C7" s="80" t="s">
@@ -3392,7 +3392,7 @@
       <c r="A8" s="48">
         <v>7</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="82" t="s">
         <v>185</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="107" t="s">
         <v>219</v>
       </c>
       <c r="C2" s="83" t="s">
@@ -3457,7 +3457,7 @@
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="77" t="s">
         <v>225</v>
       </c>
@@ -3469,7 +3469,7 @@
       <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="77" t="s">
         <v>221</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="108"/>
       <c r="C5" s="77" t="s">
         <v>222</v>
       </c>
@@ -3493,7 +3493,7 @@
       <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="107"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="77" t="s">
         <v>223</v>
       </c>
@@ -3505,7 +3505,7 @@
       <c r="A7" s="84">
         <v>6</v>
       </c>
-      <c r="B7" s="107"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="85" t="s">
         <v>224</v>
       </c>
@@ -3540,13 +3540,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3568,7 +3568,7 @@
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="109" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="83" t="s">
@@ -3582,7 +3582,7 @@
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="108"/>
+      <c r="B3" s="109"/>
       <c r="C3" s="77" t="s">
         <v>227</v>
       </c>
@@ -3594,7 +3594,7 @@
       <c r="A4" s="84">
         <v>3</v>
       </c>
-      <c r="B4" s="109"/>
+      <c r="B4" s="110"/>
       <c r="C4" s="85" t="s">
         <v>228</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="A5" s="45">
         <v>4</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="104" t="s">
         <v>229</v>
       </c>
       <c r="C5" s="79" t="s">
@@ -3620,7 +3620,7 @@
       <c r="A6" s="84">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="85" t="s">
         <v>231</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="102" t="s">
         <v>219</v>
       </c>
       <c r="C7" s="79" t="s">
@@ -3643,10 +3643,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="110">
+      <c r="A8" s="91">
         <v>7</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="82" t="s">
         <v>234</v>
       </c>

</xml_diff>

<commit_message>
Atualização Sprint backlog da semana
</commit_message>
<xml_diff>
--- a/Documentação/Project Backlog.xlsx
+++ b/Documentação/Project Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2D743F-7926-474A-BA25-316B6941CF28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDC1FA-20DA-4218-BB79-C86A69729E40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sprint Backlog (04-04)" sheetId="4" r:id="rId5"/>
     <sheet name="Sprint Backlog (09-04)" sheetId="6" r:id="rId6"/>
     <sheet name="Sprint Backlog (18-04)" sheetId="7" r:id="rId7"/>
+    <sheet name="Sprint Backlog (25-04)" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="247">
   <si>
     <t>id</t>
   </si>
@@ -740,6 +741,42 @@
   </si>
   <si>
     <t>Revisar planilha de riscos do projeto.</t>
+  </si>
+  <si>
+    <t>Ajustes Finais</t>
+  </si>
+  <si>
+    <t>Arrumar bug na tela sobre.</t>
+  </si>
+  <si>
+    <t>Arrumar bug na tela cadastro.</t>
+  </si>
+  <si>
+    <t>Colocar modal no editar galpões.</t>
+  </si>
+  <si>
+    <t>Arrumar altura do titulona tela dashboard.</t>
+  </si>
+  <si>
+    <t>Alinhar telas em tempo real.</t>
+  </si>
+  <si>
+    <t>Fazer verificação de login com sweetAlert.</t>
+  </si>
+  <si>
+    <t>Mudar cor de fundo e alinhar a tela do simulador</t>
+  </si>
+  <si>
+    <t>Adicionar botão voltar na tela de cadastro</t>
+  </si>
+  <si>
+    <t>Revisar Documentação</t>
+  </si>
+  <si>
+    <t>Apresentação</t>
+  </si>
+  <si>
+    <t>Fazer slides das apresentações</t>
   </si>
 </sst>
 </file>
@@ -855,7 +892,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1269,11 +1306,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1500,6 +1550,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3539,8 +3615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9C175-D83D-4C5E-A56D-A8DC851B7CF5}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,7 +3640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -3578,7 +3654,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>2</v>
       </c>
@@ -3590,7 +3666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="84">
         <v>3</v>
       </c>
@@ -3602,7 +3678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="45">
         <v>4</v>
       </c>
@@ -3616,7 +3692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="84">
         <v>5</v>
       </c>
@@ -3628,7 +3704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="45">
         <v>6</v>
       </c>
@@ -3662,4 +3738,167 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28B9442-EDA2-4819-BAF3-DEE835EE3CE9}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="113" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
+        <v>2</v>
+      </c>
+      <c r="B3" s="105"/>
+      <c r="C3" s="111" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="46">
+        <v>3</v>
+      </c>
+      <c r="B4" s="105"/>
+      <c r="C4" s="114" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>4</v>
+      </c>
+      <c r="B5" s="105"/>
+      <c r="C5" s="111" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="46">
+        <v>5</v>
+      </c>
+      <c r="B6" s="105"/>
+      <c r="C6" s="114" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="46">
+        <v>6</v>
+      </c>
+      <c r="B7" s="105"/>
+      <c r="C7" s="114" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="46">
+        <v>7</v>
+      </c>
+      <c r="B8" s="105"/>
+      <c r="C8" s="115" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="112" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="84">
+        <v>8</v>
+      </c>
+      <c r="B9" s="106"/>
+      <c r="C9" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="118">
+        <v>9</v>
+      </c>
+      <c r="B10" s="119" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="120" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="54">
+        <v>10</v>
+      </c>
+      <c r="B11" s="88" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="117" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:B9"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações documentação final e Manual de Instalação
</commit_message>
<xml_diff>
--- a/Documentação/Project Backlog.xlsx
+++ b/Documentação/Project Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexy\Desktop\boxzardTech\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FC3E14-AD22-47BF-BF1B-2142452FFC98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B5F53-2A02-49F4-A930-C63916C79722}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -1406,45 +1406,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1455,8 +1416,47 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1778,14 +1778,14 @@
       <selection activeCell="E2" activeCellId="3" sqref="A2 C2 D2 E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1802,11 +1802,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="71" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1819,11 +1819,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="66"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="5" t="s">
         <v>50</v>
       </c>
@@ -1834,11 +1834,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="66"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
@@ -1849,11 +1849,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1864,11 +1864,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="66"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="5" t="s">
         <v>56</v>
       </c>
@@ -1879,11 +1879,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="66"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="6" t="s">
         <v>58</v>
       </c>
@@ -1894,11 +1894,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="66"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="5" t="s">
         <v>60</v>
       </c>
@@ -1909,11 +1909,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="67"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="21" t="s">
         <v>62</v>
       </c>
@@ -1924,14 +1924,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1948,11 +1948,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="71" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1965,11 +1965,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="66"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="5" t="s">
         <v>67</v>
       </c>
@@ -1980,11 +1980,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="66"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="5" t="s">
         <v>69</v>
       </c>
@@ -1995,11 +1995,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="66"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="5" t="s">
         <v>71</v>
       </c>
@@ -2010,11 +2010,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="66"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="5" t="s">
         <v>77</v>
       </c>
@@ -2025,11 +2025,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="66"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
@@ -2040,11 +2040,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="66"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
@@ -2055,11 +2055,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="21" t="s">
         <v>75</v>
       </c>
@@ -2070,8 +2070,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -2088,11 +2088,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="71" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2105,11 +2105,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="66"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="5" t="s">
         <v>82</v>
       </c>
@@ -2120,11 +2120,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="66"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="5" t="s">
         <v>84</v>
       </c>
@@ -2135,11 +2135,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="66"/>
+      <c r="B25" s="72"/>
       <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
@@ -2150,11 +2150,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="66"/>
+      <c r="B26" s="72"/>
       <c r="C26" s="5" t="s">
         <v>88</v>
       </c>
@@ -2165,11 +2165,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="66"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
@@ -2195,18 +2195,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -2223,11 +2223,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="75" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="64" t="s">
@@ -2240,11 +2240,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="69"/>
+      <c r="B3" s="75"/>
       <c r="C3" s="6" t="s">
         <v>186</v>
       </c>
@@ -2256,11 +2256,11 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="69"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="6" t="s">
         <v>187</v>
       </c>
@@ -2272,11 +2272,11 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="69"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="6" t="s">
         <v>188</v>
       </c>
@@ -2287,11 +2287,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="69"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="6" t="s">
         <v>189</v>
       </c>
@@ -2302,11 +2302,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="28" t="s">
         <v>190</v>
       </c>
@@ -2317,18 +2317,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29"/>
       <c r="B8" s="30"/>
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="74" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2341,11 +2341,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="69"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="35" t="s">
         <v>193</v>
       </c>
@@ -2356,11 +2356,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="69"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="6" t="s">
         <v>194</v>
       </c>
@@ -2371,11 +2371,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="69"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="5" t="s">
         <v>99</v>
       </c>
@@ -2386,11 +2386,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="69"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="6" t="s">
         <v>195</v>
       </c>
@@ -2401,11 +2401,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="69"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="6" t="s">
         <v>196</v>
       </c>
@@ -2416,11 +2416,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="69"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="6" t="s">
         <v>102</v>
       </c>
@@ -2431,11 +2431,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="69"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="6" t="s">
         <v>198</v>
       </c>
@@ -2446,11 +2446,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="69"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="6" t="s">
         <v>199</v>
       </c>
@@ -2461,11 +2461,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="69"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="6" t="s">
         <v>201</v>
       </c>
@@ -2476,11 +2476,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="69"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="6" t="s">
         <v>202</v>
       </c>
@@ -2491,11 +2491,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="69"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="6" t="s">
         <v>107</v>
       </c>
@@ -2506,11 +2506,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="69"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="6" t="s">
         <v>200</v>
       </c>
@@ -2521,11 +2521,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="69"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="6" t="s">
         <v>110</v>
       </c>
@@ -2536,11 +2536,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="69"/>
+      <c r="B23" s="75"/>
       <c r="C23" s="6" t="s">
         <v>203</v>
       </c>
@@ -2551,11 +2551,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="69"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="6" t="s">
         <v>204</v>
       </c>
@@ -2566,11 +2566,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="69"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="6" t="s">
         <v>205</v>
       </c>
@@ -2581,11 +2581,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="69"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="6" t="s">
         <v>206</v>
       </c>
@@ -2596,11 +2596,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="69"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="6" t="s">
         <v>207</v>
       </c>
@@ -2611,11 +2611,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="69"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="6" t="s">
         <v>208</v>
       </c>
@@ -2626,11 +2626,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="69"/>
+      <c r="B29" s="75"/>
       <c r="C29" s="6" t="s">
         <v>209</v>
       </c>
@@ -2641,11 +2641,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="69"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="6" t="s">
         <v>210</v>
       </c>
@@ -2656,11 +2656,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="69"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="35" t="s">
         <v>118</v>
       </c>
@@ -2671,11 +2671,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="69"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="5" t="s">
         <v>211</v>
       </c>
@@ -2686,11 +2686,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="69"/>
+      <c r="B33" s="75"/>
       <c r="C33" s="6" t="s">
         <v>213</v>
       </c>
@@ -2701,11 +2701,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="69"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="5" t="s">
         <v>212</v>
       </c>
@@ -2716,11 +2716,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="69"/>
+      <c r="B35" s="75"/>
       <c r="C35" s="6" t="s">
         <v>214</v>
       </c>
@@ -2731,11 +2731,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="69"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="6" t="s">
         <v>215</v>
       </c>
@@ -2746,11 +2746,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="70"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="28" t="s">
         <v>216</v>
       </c>
@@ -2761,18 +2761,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
       <c r="D38" s="32"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="68" t="s">
+      <c r="B39" s="74" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -2785,11 +2785,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="69"/>
+      <c r="B40" s="75"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
@@ -2800,11 +2800,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="70"/>
+      <c r="B41" s="76"/>
       <c r="C41" s="21" t="s">
         <v>124</v>
       </c>
@@ -2815,18 +2815,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="37"/>
       <c r="D42" s="32"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="74" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2839,11 +2839,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="69"/>
+      <c r="B44" s="75"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2854,11 +2854,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="70"/>
+      <c r="B45" s="76"/>
       <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
@@ -2871,7 +2871,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E7" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState ref="A3:A41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A41">
     <sortCondition ref="A2"/>
   </sortState>
   <mergeCells count="4">
@@ -2889,18 +2889,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>149</v>
       </c>
@@ -2914,11 +2914,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>151</v>
       </c>
       <c r="C2" s="53" t="s">
@@ -2928,11 +2928,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="47">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="54" t="s">
         <v>153</v>
       </c>
@@ -2940,11 +2940,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A4" s="45">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="77" t="s">
         <v>154</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -2954,11 +2954,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="73"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="51" t="s">
         <v>156</v>
       </c>
@@ -2966,11 +2966,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="47">
         <v>5</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="54" t="s">
         <v>157</v>
       </c>
@@ -2978,11 +2978,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="77" t="s">
         <v>158</v>
       </c>
       <c r="C7" s="53" t="s">
@@ -2992,11 +2992,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A8" s="46">
         <v>7</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="51" t="s">
         <v>160</v>
       </c>
@@ -3004,11 +3004,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="47">
         <v>8</v>
       </c>
-      <c r="B9" s="72"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="54" t="s">
         <v>161</v>
       </c>
@@ -3016,11 +3016,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A10" s="45">
         <v>9</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="77" t="s">
         <v>162</v>
       </c>
       <c r="C10" s="53" t="s">
@@ -3030,11 +3030,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="51" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="47">
         <v>10</v>
       </c>
-      <c r="B11" s="72"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="54" t="s">
         <v>164</v>
       </c>
@@ -3042,11 +3042,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A12" s="45">
         <v>11</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="77" t="s">
         <v>165</v>
       </c>
       <c r="C12" s="53" t="s">
@@ -3056,11 +3056,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A13" s="46">
         <v>12</v>
       </c>
-      <c r="B13" s="73"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="51" t="s">
         <v>167</v>
       </c>
@@ -3068,11 +3068,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="47">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="54" t="s">
         <v>168</v>
       </c>
@@ -3081,7 +3081,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D14" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="5">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
@@ -3102,32 +3101,32 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="68" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3138,11 +3137,11 @@
       </c>
       <c r="F2" s="44"/>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="81"/>
       <c r="C3" s="12" t="s">
         <v>174</v>
       </c>
@@ -3150,11 +3149,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="84"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="12" t="s">
         <v>175</v>
       </c>
@@ -3162,11 +3161,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="84"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="12" t="s">
         <v>176</v>
       </c>
@@ -3174,11 +3173,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="12" t="s">
         <v>177</v>
       </c>
@@ -3186,11 +3185,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="84"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="12" t="s">
         <v>178</v>
       </c>
@@ -3198,11 +3197,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>8</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -3212,11 +3211,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="77"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="22" t="s">
         <v>180</v>
       </c>
@@ -3224,7 +3223,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="48"/>
       <c r="D11" s="48"/>
     </row>
@@ -3246,32 +3245,32 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="68" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3281,11 +3280,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="81"/>
       <c r="C3" s="12" t="s">
         <v>217</v>
       </c>
@@ -3293,11 +3292,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="84"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="12" t="s">
         <v>218</v>
       </c>
@@ -3305,11 +3304,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -3319,11 +3318,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="12" t="s">
         <v>183</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -3345,7 +3344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -3374,32 +3373,32 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="68" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="84" t="s">
         <v>219</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3409,11 +3408,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="12" t="s">
         <v>225</v>
       </c>
@@ -3421,11 +3420,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="12" t="s">
         <v>221</v>
       </c>
@@ -3433,11 +3432,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="75"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="12" t="s">
         <v>222</v>
       </c>
@@ -3445,11 +3444,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="12" t="s">
         <v>223</v>
       </c>
@@ -3457,11 +3456,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="12" t="s">
         <v>224</v>
       </c>
@@ -3469,11 +3468,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>7</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="70" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -3499,32 +3498,32 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="68" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="84" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3534,11 +3533,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="12" t="s">
         <v>227</v>
       </c>
@@ -3546,11 +3545,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="12" t="s">
         <v>228</v>
       </c>
@@ -3558,11 +3557,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="82" t="s">
         <v>229</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -3572,11 +3571,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="12" t="s">
         <v>231</v>
       </c>
@@ -3584,11 +3583,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="82" t="s">
         <v>219</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -3598,11 +3597,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>7</v>
       </c>
-      <c r="B8" s="77"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="22" t="s">
         <v>234</v>
       </c>
@@ -3624,36 +3623,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28B9442-EDA2-4819-BAF3-DEE835EE3CE9}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="68" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="84" t="s">
         <v>235</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3663,11 +3662,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="12" t="s">
         <v>237</v>
       </c>
@@ -3675,11 +3674,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="12" t="s">
         <v>238</v>
       </c>
@@ -3687,11 +3686,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="75"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="12" t="s">
         <v>239</v>
       </c>
@@ -3699,11 +3698,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="12" t="s">
         <v>240</v>
       </c>
@@ -3711,11 +3710,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="12" t="s">
         <v>241</v>
       </c>
@@ -3723,11 +3722,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="75"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="12" t="s">
         <v>242</v>
       </c>
@@ -3735,11 +3734,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>8</v>
       </c>
-      <c r="B9" s="75"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="12" t="s">
         <v>243</v>
       </c>
@@ -3747,11 +3746,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>9</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="69" t="s">
         <v>219</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -3761,11 +3760,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="70" t="s">
         <v>245</v>
       </c>
       <c r="C11" s="22" t="s">

</xml_diff>